<commit_message>
add checkport for 2042
Change-Id: I729b14c49a2c0baa3d54cab8ffdcef23975e6a31

Former-commit-id: 3a1413d6a9c642070c458f8876b24c36e51a0fd4
</commit_message>
<xml_diff>
--- a/SG2042EVB/config.xlsx
+++ b/SG2042EVB/config.xlsx
@@ -1963,7 +1963,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1987,7 +1987,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>EN_VDDC_B12</v>
+        <v>EN_VDD_3V3</v>
       </c>
       <c r="B2" t="str">
         <v>EN_VDD_3V3</v>
@@ -2001,7 +2001,7 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>EN_VDDC_B34</v>
+        <v>EN_VDDIO18</v>
       </c>
       <c r="B3" t="str">
         <v>EN_VDDIO18</v>
@@ -2015,7 +2015,7 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>EN_VDDC_B56</v>
+        <v>EN_VDDC</v>
       </c>
       <c r="B4" t="str">
         <v>EN_VDDC</v>
@@ -2029,38 +2029,38 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>EN_VDDC_B78</v>
+        <v>PG_VDDC</v>
       </c>
       <c r="B5" t="str">
-        <v>EN_VDDIO33</v>
+        <v>PG_VDDC</v>
       </c>
       <c r="C5" t="str">
-        <v>ENABLE</v>
+        <v>CHECK</v>
       </c>
       <c r="D5" t="str">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>EN_VDDIO33_B12</v>
+        <v>EN_VDDIO33</v>
       </c>
       <c r="B6" t="str">
-        <v>EN_DDR_VDD_0V8</v>
+        <v>EN_VDDIO33</v>
       </c>
       <c r="C6" t="str">
         <v>ENABLE</v>
       </c>
       <c r="D6" t="str">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>EN_VDDIO33_B34</v>
+        <v>EN_DDR_VDD_0V8</v>
       </c>
       <c r="B7" t="str">
-        <v>EN_VDD_PCIE_D_0V8</v>
+        <v>EN_DDR_VDD_0V8</v>
       </c>
       <c r="C7" t="str">
         <v>ENABLE</v>
@@ -2071,10 +2071,10 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>EN_VDDIO33_B56</v>
+        <v>EN_VDD_PCIE_D_0V8</v>
       </c>
       <c r="B8" t="str">
-        <v>EN_VDD_PLL_0V8</v>
+        <v>EN_VDD_PCIE_D_0V8</v>
       </c>
       <c r="C8" t="str">
         <v>ENABLE</v>
@@ -2085,27 +2085,27 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>EN_VDDIO33_B78</v>
+        <v>EN_VDD_PLL_0V8</v>
       </c>
       <c r="B9" t="str">
-        <v>EN_VDD_PCIE_H_1V8</v>
+        <v>EN_VDD_PLL_0V8</v>
       </c>
       <c r="C9" t="str">
         <v>ENABLE</v>
       </c>
       <c r="D9" t="str">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>EN_VDD_PHY_B12</v>
+        <v>PG_DDR_VDD_0V8</v>
       </c>
       <c r="B10" t="str">
-        <v>EN_DDR01_VPP_2V5</v>
+        <v>PG_DDR_VDD_0V8</v>
       </c>
       <c r="C10" t="str">
-        <v>ENABLE</v>
+        <v>CHECK</v>
       </c>
       <c r="D10" t="str">
         <v>0</v>
@@ -2113,10 +2113,10 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>EN_VDD_PHY_B34</v>
+        <v>EN_VDD_PCIE_H_1V8</v>
       </c>
       <c r="B11" t="str">
-        <v>EN_DDR23_VPP_2V5</v>
+        <v>EN_VDD_PCIE_H_1V8</v>
       </c>
       <c r="C11" t="str">
         <v>ENABLE</v>
@@ -2127,10 +2127,10 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>EN_VDD_PHY_B56</v>
+        <v>EN_DDR01_VPP_2V5</v>
       </c>
       <c r="B12" t="str">
-        <v>EN_DDR01_VDDQ_1V2</v>
+        <v>EN_DDR01_VPP_2V5</v>
       </c>
       <c r="C12" t="str">
         <v>ENABLE</v>
@@ -2141,10 +2141,10 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>EN_VDD_PHY_B78</v>
+        <v>EN_DDR23_VPP_2V5</v>
       </c>
       <c r="B13" t="str">
-        <v>EN_DDR23_VDDQ_1V2</v>
+        <v>EN_DDR23_VPP_2V5</v>
       </c>
       <c r="C13" t="str">
         <v>ENABLE</v>
@@ -2155,10 +2155,10 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>P08_PG_B12</v>
+        <v>EN_DDR01_VDDQ_1V2</v>
       </c>
       <c r="B14" t="str">
-        <v>EN_DDR01_VTT_0V6</v>
+        <v>EN_DDR01_VDDQ_1V2</v>
       </c>
       <c r="C14" t="str">
         <v>ENABLE</v>
@@ -2169,10 +2169,10 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>P08_PG_B34</v>
+        <v>EN_DDR23_VDDQ_1V2</v>
       </c>
       <c r="B15" t="str">
-        <v>EN_DDR23_VTT_0V6</v>
+        <v>EN_DDR23_VDDQ_1V2</v>
       </c>
       <c r="C15" t="str">
         <v>ENABLE</v>
@@ -2183,35 +2183,91 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>P08_PG_B56</v>
+        <v>PG_DDR01_VDDQ_1V2</v>
       </c>
       <c r="B16" t="str">
-        <v>EN_VQPS18</v>
+        <v>PG_DDR01_VDDQ_1V2</v>
       </c>
       <c r="C16" t="str">
-        <v>ENABLE</v>
+        <v>CHECK</v>
       </c>
       <c r="D16" t="str">
-        <v>30000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>P08_PG_B78</v>
+        <v>PG_DDR23_VDDQ_1V2</v>
       </c>
       <c r="B17" t="str">
+        <v>PG_DDR23_VDDQ_1V2</v>
+      </c>
+      <c r="C17" t="str">
+        <v>CHECK</v>
+      </c>
+      <c r="D17" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>EN_DDR01_VTT_0V6</v>
+      </c>
+      <c r="B18" t="str">
+        <v>EN_DDR01_VTT_0V6</v>
+      </c>
+      <c r="C18" t="str">
+        <v>ENABLE</v>
+      </c>
+      <c r="D18" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>EN_DDR23_VTT_0V6</v>
+      </c>
+      <c r="B19" t="str">
+        <v>EN_DDR23_VTT_0V6</v>
+      </c>
+      <c r="C19" t="str">
+        <v>ENABLE</v>
+      </c>
+      <c r="D19" t="str">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>EN_VQPS18</v>
+      </c>
+      <c r="B20" t="str">
+        <v>EN_VQPS18</v>
+      </c>
+      <c r="C20" t="str">
+        <v>ENABLE</v>
+      </c>
+      <c r="D20" t="str">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
         <v>SYS_RST_X_H</v>
       </c>
-      <c r="C17" t="str">
+      <c r="B21" t="str">
+        <v>SYS_RST_X_H</v>
+      </c>
+      <c r="C21" t="str">
         <v>ENABLE</v>
       </c>
-      <c r="D17" t="str">
+      <c r="D21" t="str">
         <v>1000</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E17"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E21"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
SG2042EVB:add slave:mcu and tmp451
Change-Id: I0b2f74e032bb7a1c8a11a26c41cafe4c61c1baf1

Former-commit-id: 963f111d4ecf63c91fb2b1f20f481b75ebd3b51e
</commit_message>
<xml_diff>
--- a/SG2042EVB/config.xlsx
+++ b/SG2042EVB/config.xlsx
@@ -1300,7 +1300,7 @@
         <v>PD9</v>
       </c>
       <c r="C57" t="str">
-        <v>NC</v>
+        <v>TEST_MOD</v>
       </c>
       <c r="D57" t="str">
         <v>INPUT</v>
@@ -1314,7 +1314,7 @@
         <v>PD10</v>
       </c>
       <c r="C58" t="str">
-        <v>NC</v>
+        <v>MCU_BOOT_SEL6_H</v>
       </c>
       <c r="D58" t="str">
         <v>INPUT</v>
@@ -1704,7 +1704,7 @@
         <v>PC12</v>
       </c>
       <c r="C76" t="str">
-        <v>NC</v>
+        <v>MCU_ATX_ON</v>
       </c>
       <c r="D76" t="str">
         <v>INPUT</v>
@@ -2099,30 +2099,30 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>PG_DDR_VDD_0V8</v>
+        <v>EN_VDD_PCIE_H_1V8</v>
       </c>
       <c r="B10" t="str">
-        <v>PG_DDR_VDD_0V8</v>
+        <v>EN_VDD_PCIE_H_1V8</v>
       </c>
       <c r="C10" t="str">
-        <v>CHECK</v>
+        <v>ENABLE</v>
       </c>
       <c r="D10" t="str">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>EN_VDD_PCIE_H_1V8</v>
+        <v>PG_DDR_VDD_0V8</v>
       </c>
       <c r="B11" t="str">
-        <v>EN_VDD_PCIE_H_1V8</v>
+        <v>PG_DDR_VDD_0V8</v>
       </c>
       <c r="C11" t="str">
-        <v>ENABLE</v>
+        <v>CHECK</v>
       </c>
       <c r="D11" t="str">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">

</xml_diff>

<commit_message>
SG2042EVB:complete poweron, support slt
Change-Id: Iee9a8ad50104e72e27f82b985f818ade4eebe5bd

Former-commit-id: c1f2888aeca9b51d009281985611b9c5d31f3f9e
</commit_message>
<xml_diff>
--- a/SG2042EVB/config.xlsx
+++ b/SG2042EVB/config.xlsx
@@ -8,6 +8,28 @@
     <sheet name="adc2ver" sheetId="3" r:id="rId3"/>
   </sheets>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1317,7 +1339,19 @@
         <v>MCU_BOOT_SEL6_H</v>
       </c>
       <c r="D58" t="str">
-        <v>INPUT</v>
+        <v>OUTPUT</v>
+      </c>
+      <c r="F58" t="str">
+        <v>NO-PULL</v>
+      </c>
+      <c r="G58" t="str">
+        <v>PP</v>
+      </c>
+      <c r="H58" t="str">
+        <v>LOW</v>
+      </c>
+      <c r="I58" t="str">
+        <v>0</v>
       </c>
     </row>
     <row r="59">

</xml_diff>

<commit_message>
BM1684xEVB/SG2042EVB/SG2042REVB:make changes as follow
BM1684xEVB:
	1. board temperature get from tmp451 and save in mcu
	   register(0x05)
SG2042EVB:
	1. add sys_rst into power on sequense
	2. support more information for mcu driver,such as critical
	   action, repoweron_temp...
SG2042REVB:
	1. add pwr_button into power sequence
	2. delect nct218 becauce there isn't thermal sensor link to mcu
	3. add slt as 2042rchip i2c slave, and support query slt reg from uart
	   interface
	4. support reset 2042r system from uart interface

Change-Id: I62b2a5c9dd1f99af460d1e5aa2ab19dd830a004e

Former-commit-id: 40aa90727fe05f27a47d348677a015fe1b371e6e
</commit_message>
<xml_diff>
--- a/SG2042EVB/config.xlsx
+++ b/SG2042EVB/config.xlsx
@@ -1997,7 +1997,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2287,21 +2287,35 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>SYS_RST_X_H</v>
+        <v>SYS_RST_ASSERT</v>
       </c>
       <c r="B21" t="str">
-        <v>SYS_RST_X_H</v>
+        <v>SYS_RST_ASSERT</v>
       </c>
       <c r="C21" t="str">
-        <v>ENABLE</v>
+        <v>FUNCTION</v>
       </c>
       <c r="D21" t="str">
-        <v>1000</v>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>SYS_RST_DEASSERT</v>
+      </c>
+      <c r="B22" t="str">
+        <v>SYS_RST_DEASSERT</v>
+      </c>
+      <c r="C22" t="str">
+        <v>FUNCTION</v>
+      </c>
+      <c r="D22" t="str">
+        <v>30000</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E21"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E22"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
SG2042EVB(4):support milk-v pioneer v1.1
Change-Id: Idff56eadfad6edee35403e7be77dc01515e4e5dd

Former-commit-id: bab137950530812df004af085dd3dfd7c9875dc7
</commit_message>
<xml_diff>
--- a/SG2042EVB/config.xlsx
+++ b/SG2042EVB/config.xlsx
@@ -1022,7 +1022,7 @@
         <v>PE7</v>
       </c>
       <c r="C39" t="str">
-        <v>SLOT0_PRSENT2_0</v>
+        <v>POWER_KEY</v>
       </c>
       <c r="D39" t="str">
         <v>INPUT</v>
@@ -1036,7 +1036,7 @@
         <v>PE8</v>
       </c>
       <c r="C40" t="str">
-        <v>SLOT0_PRSENT2_1</v>
+        <v>RESET_KEY</v>
       </c>
       <c r="D40" t="str">
         <v>INPUT</v>
@@ -1078,10 +1078,10 @@
         <v>PE11</v>
       </c>
       <c r="C43" t="str">
-        <v>SLOT1_PRSENT2_0</v>
+        <v>LED1</v>
       </c>
       <c r="D43" t="str">
-        <v>INPUT</v>
+        <v>OUTPUT</v>
       </c>
     </row>
     <row r="44">
@@ -1092,10 +1092,10 @@
         <v>PE12</v>
       </c>
       <c r="C44" t="str">
-        <v>SLOT1_PRSENT2_1</v>
+        <v>LED2</v>
       </c>
       <c r="D44" t="str">
-        <v>INPUT</v>
+        <v>OUTPUT</v>
       </c>
     </row>
     <row r="45">
@@ -1741,7 +1741,7 @@
         <v>MCU_ATX_ON</v>
       </c>
       <c r="D76" t="str">
-        <v>INPUT</v>
+        <v>OUTPUT</v>
       </c>
     </row>
     <row r="77">
@@ -1870,10 +1870,10 @@
         <v>PB3</v>
       </c>
       <c r="C85" t="str">
-        <v>NC</v>
+        <v>LINK_GPIO22</v>
       </c>
       <c r="D85" t="str">
-        <v>INPUT</v>
+        <v>OUTPUT</v>
       </c>
     </row>
     <row r="86">
@@ -1884,10 +1884,10 @@
         <v>PB4</v>
       </c>
       <c r="C86" t="str">
-        <v>NC</v>
+        <v>LINK_GPIO23</v>
       </c>
       <c r="D86" t="str">
-        <v>INPUT</v>
+        <v>OUTPUT</v>
       </c>
     </row>
     <row r="87">
@@ -1898,10 +1898,10 @@
         <v>PB5</v>
       </c>
       <c r="C87" t="str">
-        <v>NC</v>
+        <v>LINK_GPIO24</v>
       </c>
       <c r="D87" t="str">
-        <v>INPUT</v>
+        <v>OUTPUT</v>
       </c>
     </row>
     <row r="88">

</xml_diff>

<commit_message>
SG2042EVB(5):fixbug:pioneer system poweroff failed
Change-Id: I2ec7a609e4401aff2cb88136ed51dd7335271c95
</commit_message>
<xml_diff>
--- a/SG2042EVB/config.xlsx
+++ b/SG2042EVB/config.xlsx
@@ -1997,7 +1997,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2021,13 +2021,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>EN_VDD_3V3</v>
+        <v>MILKV_ATX_CTL</v>
       </c>
       <c r="B2" t="str">
-        <v>EN_VDD_3V3</v>
+        <v>MILKV_ATX_CTL</v>
       </c>
       <c r="C2" t="str">
-        <v>ENABLE</v>
+        <v>FUNCTION</v>
       </c>
       <c r="D2" t="str">
         <v>1000</v>
@@ -2035,10 +2035,10 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>EN_VDDIO18</v>
+        <v>EN_VDD_3V3</v>
       </c>
       <c r="B3" t="str">
-        <v>EN_VDDIO18</v>
+        <v>EN_VDD_3V3</v>
       </c>
       <c r="C3" t="str">
         <v>ENABLE</v>
@@ -2049,10 +2049,10 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>EN_VDDC</v>
+        <v>EN_VDDIO18</v>
       </c>
       <c r="B4" t="str">
-        <v>EN_VDDC</v>
+        <v>EN_VDDIO18</v>
       </c>
       <c r="C4" t="str">
         <v>ENABLE</v>
@@ -2063,52 +2063,52 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>PG_VDDC</v>
+        <v>EN_VDDC</v>
       </c>
       <c r="B5" t="str">
-        <v>PG_VDDC</v>
+        <v>EN_VDDC</v>
       </c>
       <c r="C5" t="str">
-        <v>CHECK</v>
+        <v>ENABLE</v>
       </c>
       <c r="D5" t="str">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>EN_VDDIO33</v>
+        <v>PG_VDDC</v>
       </c>
       <c r="B6" t="str">
-        <v>EN_VDDIO33</v>
+        <v>PG_VDDC</v>
       </c>
       <c r="C6" t="str">
-        <v>ENABLE</v>
+        <v>CHECK</v>
       </c>
       <c r="D6" t="str">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>EN_DDR_VDD_0V8</v>
+        <v>EN_VDDIO33</v>
       </c>
       <c r="B7" t="str">
-        <v>EN_DDR_VDD_0V8</v>
+        <v>EN_VDDIO33</v>
       </c>
       <c r="C7" t="str">
         <v>ENABLE</v>
       </c>
       <c r="D7" t="str">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>EN_VDD_PCIE_D_0V8</v>
+        <v>EN_DDR_VDD_0V8</v>
       </c>
       <c r="B8" t="str">
-        <v>EN_VDD_PCIE_D_0V8</v>
+        <v>EN_DDR_VDD_0V8</v>
       </c>
       <c r="C8" t="str">
         <v>ENABLE</v>
@@ -2119,10 +2119,10 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>EN_VDD_PLL_0V8</v>
+        <v>EN_VDD_PCIE_D_0V8</v>
       </c>
       <c r="B9" t="str">
-        <v>EN_VDD_PLL_0V8</v>
+        <v>EN_VDD_PCIE_D_0V8</v>
       </c>
       <c r="C9" t="str">
         <v>ENABLE</v>
@@ -2133,41 +2133,41 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>EN_VDD_PCIE_H_1V8</v>
+        <v>EN_VDD_PLL_0V8</v>
       </c>
       <c r="B10" t="str">
-        <v>EN_VDD_PCIE_H_1V8</v>
+        <v>EN_VDD_PLL_0V8</v>
       </c>
       <c r="C10" t="str">
         <v>ENABLE</v>
       </c>
       <c r="D10" t="str">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>PG_DDR_VDD_0V8</v>
+        <v>EN_VDD_PCIE_H_1V8</v>
       </c>
       <c r="B11" t="str">
-        <v>PG_DDR_VDD_0V8</v>
+        <v>EN_VDD_PCIE_H_1V8</v>
       </c>
       <c r="C11" t="str">
-        <v>CHECK</v>
+        <v>ENABLE</v>
       </c>
       <c r="D11" t="str">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>EN_DDR01_VPP_2V5</v>
+        <v>PG_DDR_VDD_0V8</v>
       </c>
       <c r="B12" t="str">
-        <v>EN_DDR01_VPP_2V5</v>
+        <v>PG_DDR_VDD_0V8</v>
       </c>
       <c r="C12" t="str">
-        <v>ENABLE</v>
+        <v>CHECK</v>
       </c>
       <c r="D12" t="str">
         <v>0</v>
@@ -2175,66 +2175,66 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>EN_DDR23_VPP_2V5</v>
+        <v>EN_DDR01_VPP_2V5</v>
       </c>
       <c r="B13" t="str">
-        <v>EN_DDR23_VPP_2V5</v>
+        <v>EN_DDR01_VPP_2V5</v>
       </c>
       <c r="C13" t="str">
         <v>ENABLE</v>
       </c>
       <c r="D13" t="str">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>EN_DDR01_VDDQ_1V2</v>
+        <v>EN_DDR23_VPP_2V5</v>
       </c>
       <c r="B14" t="str">
-        <v>EN_DDR01_VDDQ_1V2</v>
+        <v>EN_DDR23_VPP_2V5</v>
       </c>
       <c r="C14" t="str">
         <v>ENABLE</v>
       </c>
       <c r="D14" t="str">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>EN_DDR23_VDDQ_1V2</v>
+        <v>EN_DDR01_VDDQ_1V2</v>
       </c>
       <c r="B15" t="str">
-        <v>EN_DDR23_VDDQ_1V2</v>
+        <v>EN_DDR01_VDDQ_1V2</v>
       </c>
       <c r="C15" t="str">
         <v>ENABLE</v>
       </c>
       <c r="D15" t="str">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>PG_DDR01_VDDQ_1V2</v>
+        <v>EN_DDR23_VDDQ_1V2</v>
       </c>
       <c r="B16" t="str">
-        <v>PG_DDR01_VDDQ_1V2</v>
+        <v>EN_DDR23_VDDQ_1V2</v>
       </c>
       <c r="C16" t="str">
-        <v>CHECK</v>
+        <v>ENABLE</v>
       </c>
       <c r="D16" t="str">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>PG_DDR23_VDDQ_1V2</v>
+        <v>PG_DDR01_VDDQ_1V2</v>
       </c>
       <c r="B17" t="str">
-        <v>PG_DDR23_VDDQ_1V2</v>
+        <v>PG_DDR01_VDDQ_1V2</v>
       </c>
       <c r="C17" t="str">
         <v>CHECK</v>
@@ -2245,13 +2245,13 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>EN_DDR01_VTT_0V6</v>
+        <v>PG_DDR23_VDDQ_1V2</v>
       </c>
       <c r="B18" t="str">
-        <v>EN_DDR01_VTT_0V6</v>
+        <v>PG_DDR23_VDDQ_1V2</v>
       </c>
       <c r="C18" t="str">
-        <v>ENABLE</v>
+        <v>CHECK</v>
       </c>
       <c r="D18" t="str">
         <v>0</v>
@@ -2259,41 +2259,41 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>EN_DDR23_VTT_0V6</v>
+        <v>EN_DDR01_VTT_0V6</v>
       </c>
       <c r="B19" t="str">
-        <v>EN_DDR23_VTT_0V6</v>
+        <v>EN_DDR01_VTT_0V6</v>
       </c>
       <c r="C19" t="str">
         <v>ENABLE</v>
       </c>
       <c r="D19" t="str">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>EN_VQPS18</v>
+        <v>EN_DDR23_VTT_0V6</v>
       </c>
       <c r="B20" t="str">
-        <v>EN_VQPS18</v>
+        <v>EN_DDR23_VTT_0V6</v>
       </c>
       <c r="C20" t="str">
         <v>ENABLE</v>
       </c>
       <c r="D20" t="str">
-        <v>30000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>SYS_RST_ASSERT</v>
+        <v>EN_VQPS18</v>
       </c>
       <c r="B21" t="str">
-        <v>SYS_RST_ASSERT</v>
+        <v>EN_VQPS18</v>
       </c>
       <c r="C21" t="str">
-        <v>FUNCTION</v>
+        <v>ENABLE</v>
       </c>
       <c r="D21" t="str">
         <v>30000</v>
@@ -2301,10 +2301,10 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>SYS_RST_DEASSERT</v>
+        <v>SYS_RST_ASSERT</v>
       </c>
       <c r="B22" t="str">
-        <v>SYS_RST_DEASSERT</v>
+        <v>SYS_RST_ASSERT</v>
       </c>
       <c r="C22" t="str">
         <v>FUNCTION</v>
@@ -2313,9 +2313,23 @@
         <v>30000</v>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>SYS_RST_DEASSERT</v>
+      </c>
+      <c r="B23" t="str">
+        <v>SYS_RST_DEASSERT</v>
+      </c>
+      <c r="C23" t="str">
+        <v>FUNCTION</v>
+      </c>
+      <c r="D23" t="str">
+        <v>30000</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E22"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E23"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>